<commit_message>
Add some SpecificationSpecific things to get the sample test closer to compiling
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Rerouting.xlsx
+++ b/SampleTests/ExcelTests/Rerouting.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="120" yWindow="30" windowWidth="28620" windowHeight="12405"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Reroute to SEA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>Specification</t>
   </si>
@@ -24,9 +22,6 @@
     <t>Given a</t>
   </si>
   <si>
-    <t>With Properties</t>
-  </si>
-  <si>
     <t>RoutingService</t>
   </si>
   <si>
@@ -51,18 +46,6 @@
     <t>DAL</t>
   </si>
   <si>
-    <t>Itinerary</t>
-  </si>
-  <si>
-    <t>Itinerary of</t>
-  </si>
-  <si>
-    <t>Leg table of</t>
-  </si>
-  <si>
-    <t>Leg</t>
-  </si>
-  <si>
     <t>LGB</t>
   </si>
   <si>
@@ -85,6 +68,15 @@
   </si>
   <si>
     <t>Reroute to SEA</t>
+  </si>
+  <si>
+    <t>Reroute From of</t>
+  </si>
+  <si>
+    <t>ItineraryLeg table of</t>
+  </si>
+  <si>
+    <t>ItineraryLeg</t>
   </si>
 </sst>
 </file>
@@ -168,7 +160,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,6 +176,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
@@ -193,8 +188,36 @@
     <cellStyle name="Accent4" xfId="1" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -490,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,218 +525,161 @@
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="C7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="D8" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="F10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F12" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="D7" s="8" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="7" t="s">
+      <c r="G13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" s="5" t="s">
-        <v>15</v>
-      </c>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Arrange and act parts of the test compile now, need to work on the assert bit
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Rerouting.xlsx
+++ b/SampleTests/ExcelTests/Rerouting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Specification</t>
   </si>
@@ -52,9 +52,6 @@
     <t>SEA</t>
   </si>
   <si>
-    <t>Reroute To of</t>
-  </si>
-  <si>
     <t>When</t>
   </si>
   <si>
@@ -70,13 +67,19 @@
     <t>Reroute to SEA</t>
   </si>
   <si>
-    <t>Reroute From of</t>
-  </si>
-  <si>
     <t>ItineraryLeg table of</t>
   </si>
   <si>
     <t>ItineraryLeg</t>
+  </si>
+  <si>
+    <t>RerouteFrom of</t>
+  </si>
+  <si>
+    <t>RerouteTo of</t>
+  </si>
+  <si>
+    <t>With Properties</t>
   </si>
 </sst>
 </file>
@@ -173,12 +176,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
@@ -516,7 +519,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +529,7 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -536,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -550,25 +553,25 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>11</v>
@@ -583,10 +586,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="D8" s="8" t="s">
-        <v>4</v>
+      <c r="D8" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,16 +609,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E11" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="F12" s="8" t="s">
-        <v>4</v>
+      <c r="E11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F12" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -644,22 +647,22 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Manually fix up test, which now passes. Need to fix up code generate to create the code in this way
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Rerouting.xlsx
+++ b/SampleTests/ExcelTests/Rerouting.xlsx
@@ -64,9 +64,6 @@
     <t>Rerouted Cargo</t>
   </si>
   <si>
-    <t>Reroute to SEA</t>
-  </si>
-  <si>
     <t>ItineraryLeg table of</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>With Properties</t>
+  </si>
+  <si>
+    <t>Reroute To Sea</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -561,7 +561,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>9</v>
@@ -571,7 +571,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>11</v>
@@ -589,7 +589,7 @@
     <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="D8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -610,15 +610,15 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add usings and assertionClassPrefix parameters to c# code generator, fix up excel file and sut so that test works
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Rerouting.xlsx
+++ b/SampleTests/ExcelTests/Rerouting.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="120" yWindow="30" windowWidth="28620" windowHeight="12405"/>
   </bookViews>
   <sheets>
-    <sheet name="Reroute to SEA" sheetId="1" r:id="rId1"/>
+    <sheet name="Reroute To Sea" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Specification</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Assert</t>
   </si>
   <si>
-    <t>Rerouted Cargo</t>
-  </si>
-  <si>
     <t>ItineraryLeg table of</t>
   </si>
   <si>
@@ -79,7 +76,19 @@
     <t>With Properties</t>
   </si>
   <si>
-    <t>Reroute To Sea</t>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Reroute Cargo from HKG - DAL to HKG - SEA</t>
   </si>
 </sst>
 </file>
@@ -163,7 +172,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -181,6 +190,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +551,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3"/>
     </row>
@@ -561,7 +573,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>9</v>
@@ -571,7 +583,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>11</v>
@@ -589,7 +601,7 @@
     <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="D8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -610,15 +622,15 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -645,40 +657,46 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="10" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="5" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="5" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove feature to set up constructor properties
This makes the generated code easier to read and the algorithm easier to read. Constructor properties aren't really used or required so there isn't much loss. Generally you will set up interfaces in tests, and then use a test adapter of some kind to instantiate the system under test, and this test adapter can pass the relevant thiings in to the constructor
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Rerouting.xlsx
+++ b/SampleTests/ExcelTests/Rerouting.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Specification</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>Cargo</t>
-  </si>
-  <si>
-    <t>With Creational</t>
   </si>
   <si>
     <t>Origin of</t>
@@ -531,7 +528,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,9 +548,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -566,33 +564,33 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="11" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="C7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>3</v>
@@ -601,78 +599,78 @@
     <row r="8" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="D8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F14" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>3</v>
@@ -680,24 +678,24 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>22</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add check for non round trippable excel
And do some minor code tidy up

The generated code will now contain a property to state
whether it is round trippable or not, and another to state
the issues that are preventing round trips.

Currently only one test is made, which is for a blank line
between the given and when sections
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Rerouting.xlsx
+++ b/SampleTests/ExcelTests/Rerouting.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D469124-4420-494C-9726-24394873421F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0CAA1053-1B52-4B2A-8E34-CDC7E5E33DD5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="One Way Anova" sheetId="1" r:id="rId1"/>
+    <sheet name="Reroute To Sea" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -134,89 +134,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>

</xml_diff>